<commit_message>
Started to parse data
</commit_message>
<xml_diff>
--- a/Furbish Index vol 1-14.xlsx
+++ b/Furbish Index vol 1-14.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27426"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27715"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kstefko/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/sardell/public_html/furbish_project/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5420" yWindow="460" windowWidth="10000" windowHeight="15600"/>
+    <workbookView xWindow="1100" yWindow="460" windowWidth="16300" windowHeight="16760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8840" uniqueCount="3845">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8842" uniqueCount="3847">
   <si>
     <t>Volume</t>
   </si>
@@ -11586,6 +11586,12 @@
   </si>
   <si>
     <t>tall sunflower</t>
+  </si>
+  <si>
+    <t>Place Name-9</t>
+  </si>
+  <si>
+    <t>Year-9</t>
   </si>
 </sst>
 </file>
@@ -12714,9 +12720,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y1369"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A525" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I532" sqref="I532"/>
+    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="W7" sqref="W7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -12744,10 +12750,11 @@
     <col min="21" max="21" width="10" style="1" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="15.5" style="1" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="16384" width="8.83203125" style="1"/>
+    <col min="24" max="25" width="11.6640625" style="1" customWidth="1"/>
+    <col min="26" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -12817,8 +12824,14 @@
       <c r="W1" s="2" t="s">
         <v>687</v>
       </c>
-    </row>
-    <row r="2" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X1" s="2" t="s">
+        <v>3845</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>3846</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B2" s="3">
         <v>1</v>
       </c>
@@ -12847,7 +12860,7 @@
         <v>1881</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -12885,7 +12898,7 @@
         <v>1891</v>
       </c>
     </row>
-    <row r="4" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:25" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>1</v>
       </c>
@@ -12911,7 +12924,7 @@
         <v>1881</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>1</v>
       </c>
@@ -12943,7 +12956,7 @@
         <v>1878</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>1</v>
       </c>
@@ -12990,7 +13003,7 @@
         <v>1892</v>
       </c>
     </row>
-    <row r="7" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:25" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>1</v>
       </c>
@@ -13013,7 +13026,7 @@
         <v>1881</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>1</v>
       </c>
@@ -13045,7 +13058,7 @@
         <v>1897</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>1</v>
       </c>
@@ -13092,7 +13105,7 @@
         <v>1898</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>1</v>
       </c>
@@ -13136,7 +13149,7 @@
         <v>1893</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>1</v>
       </c>
@@ -13162,7 +13175,7 @@
         <v>1995</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>1</v>
       </c>
@@ -13188,7 +13201,7 @@
         <v>1886</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>1</v>
       </c>
@@ -13226,7 +13239,7 @@
         <v>1895</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>1</v>
       </c>
@@ -13270,7 +13283,7 @@
         <v>1898</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>1</v>
       </c>
@@ -13314,7 +13327,7 @@
         <v>1898</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>1</v>
       </c>

</xml_diff>